<commit_message>
added after day 6
</commit_message>
<xml_diff>
--- a/JAVA Virtual Training Plan.xlsx
+++ b/JAVA Virtual Training Plan.xlsx
@@ -1072,11 +1072,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:F19"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9:F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="9" style="19"/>
     <col min="2" max="2" width="21.25" style="19" customWidth="1"/>
@@ -1086,7 +1086,7 @@
     <col min="6" max="6" width="46.625" style="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="45" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:6" ht="45.4" x14ac:dyDescent="1.2">
       <c r="A1" s="23" t="s">
         <v>69</v>
       </c>
@@ -1096,7 +1096,7 @@
       <c r="E1" s="24"/>
       <c r="F1" s="24"/>
     </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="21" t="s">
         <v>0</v>
       </c>
@@ -1110,7 +1110,7 @@
       <c r="E2" s="25"/>
       <c r="F2" s="25"/>
     </row>
-    <row r="3" spans="1:6" ht="63.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="63.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="20">
         <v>1</v>
       </c>
@@ -1126,7 +1126,7 @@
       </c>
       <c r="F3" s="36"/>
     </row>
-    <row r="4" spans="1:6" ht="99" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="99" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1142,7 +1142,7 @@
       </c>
       <c r="F4" s="38"/>
     </row>
-    <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.35">
       <c r="A5" s="4">
         <v>3</v>
       </c>
@@ -1162,7 +1162,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="105" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="105" x14ac:dyDescent="0.35">
       <c r="A6" s="7">
         <v>4</v>
       </c>
@@ -1182,7 +1182,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="105" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="105" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1202,7 +1202,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="105" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="105" x14ac:dyDescent="0.35">
       <c r="A8" s="9">
         <v>6</v>
       </c>
@@ -1222,7 +1222,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.35">
       <c r="A9" s="4">
         <v>7</v>
       </c>
@@ -1242,7 +1242,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="60" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="60" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1262,7 +1262,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="90" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="90" x14ac:dyDescent="0.35">
       <c r="A11" s="4">
         <v>9</v>
       </c>
@@ -1282,7 +1282,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="61.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" ht="61.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1298,7 +1298,7 @@
       </c>
       <c r="F12" s="33"/>
     </row>
-    <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="11">
         <v>11</v>
       </c>
@@ -1310,7 +1310,7 @@
       <c r="E13" s="35"/>
       <c r="F13" s="11"/>
     </row>
-    <row r="14" spans="1:6" ht="60" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.35">
       <c r="A14" s="12">
         <v>12</v>
       </c>
@@ -1330,7 +1330,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="75" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" ht="75" x14ac:dyDescent="0.4">
       <c r="A15" s="14">
         <v>13</v>
       </c>
@@ -1348,7 +1348,7 @@
       </c>
       <c r="F15" s="34"/>
     </row>
-    <row r="16" spans="1:6" ht="63" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" ht="60" x14ac:dyDescent="0.35">
       <c r="A16" s="14">
         <v>14</v>
       </c>
@@ -1364,7 +1364,7 @@
       </c>
       <c r="F16" s="27"/>
     </row>
-    <row r="17" spans="1:6" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="38.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="16">
         <v>15</v>
       </c>
@@ -1380,7 +1380,7 @@
       </c>
       <c r="F17" s="30"/>
     </row>
-    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.35">
       <c r="A18" s="16">
         <v>16</v>
       </c>
@@ -1400,7 +1400,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.35">
       <c r="A19" s="16">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
added files after day 11
</commit_message>
<xml_diff>
--- a/JAVA Virtual Training Plan.xlsx
+++ b/JAVA Virtual Training Plan.xlsx
@@ -1072,8 +1072,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:F11"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.4"/>
@@ -1298,7 +1298,7 @@
       </c>
       <c r="F12" s="33"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="11">
         <v>11</v>
       </c>
@@ -1308,7 +1308,7 @@
       <c r="C13" s="35"/>
       <c r="D13" s="35"/>
       <c r="E13" s="35"/>
-      <c r="F13" s="11"/>
+      <c r="F13" s="35"/>
     </row>
     <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.35">
       <c r="A14" s="12">
@@ -1429,12 +1429,12 @@
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="E12:F12"/>
     <mergeCell ref="E15:F15"/>
-    <mergeCell ref="B13:E13"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="C4:D4"/>
+    <mergeCell ref="B13:F13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
after day 13 session
</commit_message>
<xml_diff>
--- a/JAVA Virtual Training Plan.xlsx
+++ b/JAVA Virtual Training Plan.xlsx
@@ -256,7 +256,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -302,13 +302,6 @@
       <scheme val="major"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF9C6500"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="major"/>
-    </font>
-    <font>
       <b/>
       <sz val="36"/>
       <color rgb="FF000000"/>
@@ -323,7 +316,7 @@
       <scheme val="major"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -347,6 +340,12 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="17">
     <border>
@@ -559,7 +558,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -598,21 +597,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -620,36 +604,15 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -657,9 +620,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -669,6 +629,51 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1073,58 +1078,58 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="9" style="19"/>
-    <col min="2" max="2" width="21.25" style="19" customWidth="1"/>
-    <col min="3" max="3" width="31.375" style="19" customWidth="1"/>
-    <col min="4" max="4" width="36.375" style="19" customWidth="1"/>
-    <col min="5" max="5" width="40.25" style="19" customWidth="1"/>
-    <col min="6" max="6" width="46.625" style="19" customWidth="1"/>
+    <col min="1" max="1" width="9" style="14"/>
+    <col min="2" max="2" width="21.25" style="14" customWidth="1"/>
+    <col min="3" max="3" width="31.375" style="14" customWidth="1"/>
+    <col min="4" max="4" width="36.375" style="14" customWidth="1"/>
+    <col min="5" max="5" width="40.25" style="14" customWidth="1"/>
+    <col min="6" max="6" width="46.625" style="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="45.4" x14ac:dyDescent="1.2">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
     </row>
     <row r="3" spans="1:6" ht="63.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="20">
+      <c r="A3" s="15">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="D3" s="34"/>
-      <c r="E3" s="36" t="s">
+      <c r="D3" s="22"/>
+      <c r="E3" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="36"/>
+      <c r="F3" s="23"/>
     </row>
     <row r="4" spans="1:6" ht="99" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
@@ -1133,14 +1138,14 @@
       <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="37" t="s">
+      <c r="C4" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="38"/>
-      <c r="E4" s="37" t="s">
+      <c r="D4" s="25"/>
+      <c r="E4" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="38"/>
+      <c r="F4" s="25"/>
     </row>
     <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.35">
       <c r="A5" s="4">
@@ -1289,26 +1294,26 @@
       <c r="B12" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="32" t="s">
+      <c r="C12" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="33"/>
-      <c r="E12" s="32" t="s">
+      <c r="D12" s="21"/>
+      <c r="E12" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="F12" s="33"/>
+      <c r="F12" s="21"/>
     </row>
     <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="11">
         <v>11</v>
       </c>
-      <c r="B13" s="35" t="s">
+      <c r="B13" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="C13" s="35"/>
-      <c r="D13" s="35"/>
-      <c r="E13" s="35"/>
-      <c r="F13" s="35"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
     </row>
     <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.35">
       <c r="A14" s="12">
@@ -1331,90 +1336,90 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="75" x14ac:dyDescent="0.4">
-      <c r="A15" s="14">
+      <c r="A15" s="27">
         <v>13</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="D15" s="15" t="s">
+      <c r="D15" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="E15" s="34" t="s">
+      <c r="E15" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="F15" s="34"/>
+      <c r="F15" s="30"/>
     </row>
     <row r="16" spans="1:6" ht="60" x14ac:dyDescent="0.35">
-      <c r="A16" s="14">
+      <c r="A16" s="27">
         <v>14</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="C16" s="26" t="s">
+      <c r="C16" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="D16" s="27"/>
-      <c r="E16" s="28" t="s">
+      <c r="D16" s="32"/>
+      <c r="E16" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="F16" s="27"/>
+      <c r="F16" s="32"/>
     </row>
     <row r="17" spans="1:6" ht="38.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="16">
+      <c r="A17" s="34">
         <v>15</v>
       </c>
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="C17" s="29" t="s">
+      <c r="C17" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="D17" s="30"/>
-      <c r="E17" s="31" t="s">
+      <c r="D17" s="37"/>
+      <c r="E17" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="F17" s="30"/>
+      <c r="F17" s="37"/>
     </row>
     <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.35">
-      <c r="A18" s="16">
+      <c r="A18" s="34">
         <v>16</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="C18" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="D18" s="17" t="s">
+      <c r="D18" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="E18" s="17" t="s">
+      <c r="E18" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="F18" s="17" t="s">
+      <c r="F18" s="35" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.35">
-      <c r="A19" s="16">
+      <c r="A19" s="34">
         <v>17</v>
       </c>
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="39" t="s">
         <v>53</v>
       </c>
-      <c r="C19" s="18" t="s">
+      <c r="C19" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="D19" s="22" t="s">
+      <c r="D19" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="E19" s="22"/>
-      <c r="F19" s="18" t="s">
+      <c r="E19" s="40"/>
+      <c r="F19" s="39" t="s">
         <v>62</v>
       </c>
     </row>

</xml_diff>